<commit_message>
Adds exception handling for invalid excell data input.
</commit_message>
<xml_diff>
--- a/MoneyManagerUI/MMData.xlsx
+++ b/MoneyManagerUI/MMData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Transport" sheetId="1" r:id="rId1"/>
@@ -100,11 +100,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -387,19 +389,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -413,7 +416,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>20</v>
       </c>
       <c r="B2" s="2">
@@ -436,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>